<commit_message>
Added räksmörgås.josefsson.org as example domain
</commit_message>
<xml_diff>
--- a/domains/domains.xlsx
+++ b/domains/domains.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t xml:space="preserve">University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">räksmörgås.josefsson.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
   </si>
 </sst>
 </file>
@@ -186,38 +195,37 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,10 +328,24 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>